<commit_message>
updates answers dataset with corrected data
</commit_message>
<xml_diff>
--- a/src/technology/tutorial-basic/answers/answers.xlsx
+++ b/src/technology/tutorial-basic/answers/answers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rhanes\GitHub\tyche\src\technology\tutorial-basic\answers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3A627EFE-81CF-4750-B6FE-1C7CC3DBA3EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{580F3EFC-5DE6-4654-A71F-B54C8EBCD269}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2745" yWindow="1815" windowWidth="20910" windowHeight="11775" xr2:uid="{A613468B-4246-47D0-8059-797BD75C3238}"/>
+    <workbookView xWindow="29970" yWindow="-6090" windowWidth="12150" windowHeight="21285" activeTab="2" xr2:uid="{A613468B-4246-47D0-8059-797BD75C3238}"/>
   </bookViews>
   <sheets>
     <sheet name="designs" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1019" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1007" uniqueCount="118">
   <si>
     <t>Technology</t>
   </si>
@@ -234,24 +234,6 @@
   </si>
   <si>
     <t>Foundations, roads, civil work.</t>
-  </si>
-  <si>
-    <t>Replacements</t>
-  </si>
-  <si>
-    <t>Replacement components.</t>
-  </si>
-  <si>
-    <t>O&amp;M</t>
-  </si>
-  <si>
-    <t>Operations and maintenance.</t>
-  </si>
-  <si>
-    <t>Land</t>
-  </si>
-  <si>
-    <t>Land lease.</t>
   </si>
   <si>
     <t>Just a placeholder because at least one input is required.</t>
@@ -767,7 +749,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{404BF247-5429-4E4B-9678-6277797CABB5}">
   <dimension ref="A1:G101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -3163,9 +3145,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC5423B8-8C49-451E-B763-E5AF0240ECDF}">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -3262,16 +3246,16 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>48</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>64</v>
+        <v>22</v>
       </c>
       <c r="D6">
         <v>0</v>
       </c>
       <c r="E6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -3279,16 +3263,16 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>48</v>
+        <v>65</v>
       </c>
       <c r="C7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7" t="s">
         <v>66</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -3296,13 +3280,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>48</v>
+        <v>67</v>
       </c>
       <c r="C8" t="s">
         <v>68</v>
       </c>
       <c r="D8">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E8" t="s">
         <v>69</v>
@@ -3313,16 +3297,16 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>67</v>
       </c>
       <c r="C9" t="s">
-        <v>22</v>
+        <v>70</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -3330,16 +3314,16 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>72</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E10" t="s">
-        <v>72</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -3347,67 +3331,16 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C11" t="s">
         <v>73</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11">
+        <v>3</v>
+      </c>
+      <c r="E11" t="s">
         <v>74</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" t="s">
-        <v>73</v>
-      </c>
-      <c r="C12" t="s">
-        <v>76</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" t="s">
-        <v>73</v>
-      </c>
-      <c r="C13" t="s">
-        <v>78</v>
-      </c>
-      <c r="D13">
-        <v>2</v>
-      </c>
-      <c r="E13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" t="s">
-        <v>73</v>
-      </c>
-      <c r="C14" t="s">
-        <v>79</v>
-      </c>
-      <c r="D14">
-        <v>3</v>
-      </c>
-      <c r="E14" t="s">
-        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -3425,13 +3358,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B1" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C1" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D1" t="s">
         <v>6</v>
@@ -3439,35 +3372,35 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="B2" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C2" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="B3" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C3" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C4" t="s">
         <v>84</v>
-      </c>
-      <c r="B4" t="s">
-        <v>89</v>
-      </c>
-      <c r="C4" t="s">
-        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -3491,7 +3424,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="D1" t="s">
         <v>58</v>
@@ -3514,7 +3447,7 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -3526,7 +3459,7 @@
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -3537,7 +3470,7 @@
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -3549,7 +3482,7 @@
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -3560,7 +3493,7 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -3572,7 +3505,7 @@
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -3583,7 +3516,7 @@
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D5">
         <v>3</v>
@@ -3595,7 +3528,7 @@
         <v>1</v>
       </c>
       <c r="G5" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -3606,7 +3539,7 @@
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D6">
         <v>4</v>
@@ -3618,7 +3551,7 @@
         <v>1</v>
       </c>
       <c r="G6" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -3629,19 +3562,19 @@
         <v>36</v>
       </c>
       <c r="C7" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="D7">
         <v>0</v>
       </c>
       <c r="E7" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="F7">
         <v>1</v>
       </c>
       <c r="G7" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -3652,7 +3585,7 @@
         <v>36</v>
       </c>
       <c r="C8" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -3664,7 +3597,7 @@
         <v>1</v>
       </c>
       <c r="G8" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -3675,7 +3608,7 @@
         <v>36</v>
       </c>
       <c r="C9" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="D9">
         <v>2</v>
@@ -3687,7 +3620,7 @@
         <v>1</v>
       </c>
       <c r="G9" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -3698,7 +3631,7 @@
         <v>36</v>
       </c>
       <c r="C10" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D10">
         <v>3</v>
@@ -3710,7 +3643,7 @@
         <v>1</v>
       </c>
       <c r="G10" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -3721,7 +3654,7 @@
         <v>36</v>
       </c>
       <c r="C11" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D11">
         <v>4</v>
@@ -3733,7 +3666,7 @@
         <v>1</v>
       </c>
       <c r="G11" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -3744,19 +3677,19 @@
         <v>37</v>
       </c>
       <c r="C12" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="D12">
         <v>0</v>
       </c>
       <c r="E12" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="F12">
         <v>1</v>
       </c>
       <c r="G12" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -3767,7 +3700,7 @@
         <v>37</v>
       </c>
       <c r="C13" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -3779,7 +3712,7 @@
         <v>1</v>
       </c>
       <c r="G13" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -3790,7 +3723,7 @@
         <v>37</v>
       </c>
       <c r="C14" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="D14">
         <v>2</v>
@@ -3802,7 +3735,7 @@
         <v>1</v>
       </c>
       <c r="G14" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -3813,7 +3746,7 @@
         <v>37</v>
       </c>
       <c r="C15" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D15">
         <v>3</v>
@@ -3825,7 +3758,7 @@
         <v>1</v>
       </c>
       <c r="G15" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -3836,7 +3769,7 @@
         <v>37</v>
       </c>
       <c r="C16" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D16">
         <v>4</v>
@@ -3848,7 +3781,7 @@
         <v>1</v>
       </c>
       <c r="G16" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -3859,19 +3792,19 @@
         <v>38</v>
       </c>
       <c r="C17" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="D17">
         <v>0</v>
       </c>
       <c r="E17" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="F17">
         <v>1</v>
       </c>
       <c r="G17" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -3882,7 +3815,7 @@
         <v>38</v>
       </c>
       <c r="C18" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -3894,7 +3827,7 @@
         <v>1</v>
       </c>
       <c r="G18" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -3905,7 +3838,7 @@
         <v>38</v>
       </c>
       <c r="C19" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="D19">
         <v>2</v>
@@ -3917,7 +3850,7 @@
         <v>1</v>
       </c>
       <c r="G19" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -3928,7 +3861,7 @@
         <v>38</v>
       </c>
       <c r="C20" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D20">
         <v>3</v>
@@ -3940,7 +3873,7 @@
         <v>1</v>
       </c>
       <c r="G20" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -3951,7 +3884,7 @@
         <v>38</v>
       </c>
       <c r="C21" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D21">
         <v>4</v>
@@ -3963,7 +3896,7 @@
         <v>1</v>
       </c>
       <c r="G21" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -3974,7 +3907,7 @@
         <v>39</v>
       </c>
       <c r="C22" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="D22">
         <v>0</v>
@@ -3986,7 +3919,7 @@
         <v>1</v>
       </c>
       <c r="G22" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -3997,19 +3930,19 @@
         <v>39</v>
       </c>
       <c r="C23" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="D23">
         <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="F23">
         <v>1</v>
       </c>
       <c r="G23" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -4020,7 +3953,7 @@
         <v>39</v>
       </c>
       <c r="C24" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="D24">
         <v>2</v>
@@ -4032,7 +3965,7 @@
         <v>1</v>
       </c>
       <c r="G24" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -4043,7 +3976,7 @@
         <v>39</v>
       </c>
       <c r="C25" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D25">
         <v>3</v>
@@ -4055,7 +3988,7 @@
         <v>1</v>
       </c>
       <c r="G25" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -4066,7 +3999,7 @@
         <v>39</v>
       </c>
       <c r="C26" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D26">
         <v>4</v>
@@ -4078,7 +4011,7 @@
         <v>1</v>
       </c>
       <c r="G26" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -4089,7 +4022,7 @@
         <v>40</v>
       </c>
       <c r="C27" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="D27">
         <v>0</v>
@@ -4101,7 +4034,7 @@
         <v>1</v>
       </c>
       <c r="G27" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -4112,19 +4045,19 @@
         <v>40</v>
       </c>
       <c r="C28" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="D28">
         <v>1</v>
       </c>
       <c r="E28" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="F28">
         <v>1</v>
       </c>
       <c r="G28" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -4135,7 +4068,7 @@
         <v>40</v>
       </c>
       <c r="C29" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="D29">
         <v>2</v>
@@ -4147,7 +4080,7 @@
         <v>1</v>
       </c>
       <c r="G29" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -4158,7 +4091,7 @@
         <v>40</v>
       </c>
       <c r="C30" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D30">
         <v>3</v>
@@ -4170,7 +4103,7 @@
         <v>1</v>
       </c>
       <c r="G30" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -4181,7 +4114,7 @@
         <v>40</v>
       </c>
       <c r="C31" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D31">
         <v>4</v>
@@ -4193,7 +4126,7 @@
         <v>1</v>
       </c>
       <c r="G31" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -4204,7 +4137,7 @@
         <v>41</v>
       </c>
       <c r="C32" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="D32">
         <v>0</v>
@@ -4216,7 +4149,7 @@
         <v>1</v>
       </c>
       <c r="G32" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -4227,19 +4160,19 @@
         <v>41</v>
       </c>
       <c r="C33" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="D33">
         <v>1</v>
       </c>
       <c r="E33" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="F33">
         <v>1</v>
       </c>
       <c r="G33" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -4250,7 +4183,7 @@
         <v>41</v>
       </c>
       <c r="C34" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="D34">
         <v>2</v>
@@ -4262,7 +4195,7 @@
         <v>1</v>
       </c>
       <c r="G34" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -4273,7 +4206,7 @@
         <v>41</v>
       </c>
       <c r="C35" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D35">
         <v>3</v>
@@ -4285,7 +4218,7 @@
         <v>1</v>
       </c>
       <c r="G35" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -4296,7 +4229,7 @@
         <v>41</v>
       </c>
       <c r="C36" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D36">
         <v>4</v>
@@ -4308,7 +4241,7 @@
         <v>1</v>
       </c>
       <c r="G36" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -4319,7 +4252,7 @@
         <v>42</v>
       </c>
       <c r="C37" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="D37">
         <v>0</v>
@@ -4331,7 +4264,7 @@
         <v>1</v>
       </c>
       <c r="G37" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -4342,7 +4275,7 @@
         <v>42</v>
       </c>
       <c r="C38" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="D38">
         <v>1</v>
@@ -4354,7 +4287,7 @@
         <v>1</v>
       </c>
       <c r="G38" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -4365,19 +4298,19 @@
         <v>42</v>
       </c>
       <c r="C39" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="D39">
         <v>2</v>
       </c>
       <c r="E39" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="F39">
         <v>1</v>
       </c>
       <c r="G39" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -4388,7 +4321,7 @@
         <v>42</v>
       </c>
       <c r="C40" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D40">
         <v>3</v>
@@ -4400,7 +4333,7 @@
         <v>1</v>
       </c>
       <c r="G40" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -4411,7 +4344,7 @@
         <v>42</v>
       </c>
       <c r="C41" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D41">
         <v>4</v>
@@ -4423,7 +4356,7 @@
         <v>1</v>
       </c>
       <c r="G41" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -4434,7 +4367,7 @@
         <v>43</v>
       </c>
       <c r="C42" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="D42">
         <v>0</v>
@@ -4446,7 +4379,7 @@
         <v>1</v>
       </c>
       <c r="G42" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -4457,7 +4390,7 @@
         <v>43</v>
       </c>
       <c r="C43" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="D43">
         <v>1</v>
@@ -4469,7 +4402,7 @@
         <v>1</v>
       </c>
       <c r="G43" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -4480,19 +4413,19 @@
         <v>43</v>
       </c>
       <c r="C44" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="D44">
         <v>2</v>
       </c>
       <c r="E44" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="F44">
         <v>1</v>
       </c>
       <c r="G44" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
@@ -4503,7 +4436,7 @@
         <v>43</v>
       </c>
       <c r="C45" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D45">
         <v>3</v>
@@ -4515,7 +4448,7 @@
         <v>1</v>
       </c>
       <c r="G45" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
@@ -4526,7 +4459,7 @@
         <v>43</v>
       </c>
       <c r="C46" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D46">
         <v>4</v>
@@ -4538,7 +4471,7 @@
         <v>1</v>
       </c>
       <c r="G46" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
@@ -4549,7 +4482,7 @@
         <v>44</v>
       </c>
       <c r="C47" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="D47">
         <v>0</v>
@@ -4561,7 +4494,7 @@
         <v>1</v>
       </c>
       <c r="G47" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
@@ -4572,7 +4505,7 @@
         <v>44</v>
       </c>
       <c r="C48" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="D48">
         <v>1</v>
@@ -4584,7 +4517,7 @@
         <v>1</v>
       </c>
       <c r="G48" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
@@ -4595,19 +4528,19 @@
         <v>44</v>
       </c>
       <c r="C49" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="D49">
         <v>2</v>
       </c>
       <c r="E49" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="F49">
         <v>1</v>
       </c>
       <c r="G49" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
@@ -4618,7 +4551,7 @@
         <v>44</v>
       </c>
       <c r="C50" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D50">
         <v>3</v>
@@ -4630,7 +4563,7 @@
         <v>1</v>
       </c>
       <c r="G50" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
@@ -4641,7 +4574,7 @@
         <v>44</v>
       </c>
       <c r="C51" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D51">
         <v>4</v>
@@ -4653,7 +4586,7 @@
         <v>1</v>
       </c>
       <c r="G51" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -4691,13 +4624,13 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C2" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="D2" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -4705,13 +4638,13 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C3" t="s">
         <v>31</v>
       </c>
       <c r="D3" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -4719,13 +4652,13 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C4" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="D4" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -4733,13 +4666,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C5" t="s">
         <v>73</v>
       </c>
-      <c r="C5" t="s">
-        <v>79</v>
-      </c>
       <c r="D5" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -4747,10 +4680,10 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C6" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D6" t="s">
         <v>34</v>
@@ -4761,10 +4694,10 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C7" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="D7" t="s">
         <v>11</v>
@@ -4785,16 +4718,16 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B1" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="E1" t="s">
         <v>6</v>
@@ -4802,10 +4735,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B2" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
@@ -4816,10 +4749,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B3" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="C3" t="s">
         <v>36</v>
@@ -4830,10 +4763,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B4" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C4" t="s">
         <v>37</v>
@@ -4844,10 +4777,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B5" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="C5" t="s">
         <v>38</v>
@@ -4858,10 +4791,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B6" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
@@ -4872,10 +4805,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B7" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="C7" t="s">
         <v>39</v>
@@ -4886,10 +4819,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B8" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="C8" t="s">
         <v>40</v>
@@ -4900,10 +4833,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B9" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="C9" t="s">
         <v>41</v>
@@ -4914,10 +4847,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B10" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="C10" t="s">
         <v>8</v>
@@ -4928,10 +4861,10 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B11" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="C11" t="s">
         <v>42</v>
@@ -4942,10 +4875,10 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B12" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="C12" t="s">
         <v>43</v>
@@ -4956,10 +4889,10 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B13" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="C13" t="s">
         <v>44</v>

</xml_diff>